<commit_message>
Converted all PURE components to µM
</commit_message>
<xml_diff>
--- a/modeling/PURE Formulations.xlsx
+++ b/modeling/PURE Formulations.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleclourenco/Desktop/REU-2017-Endy-Lab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleclourenco/Desktop/REU-2017-Endy-Lab/engineering/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="460" windowWidth="21700" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="21700" windowHeight="16120" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Literature PURE" sheetId="1" r:id="rId1"/>
-    <sheet name="tRNA Abundances E. coli" sheetId="2" r:id="rId2"/>
+    <sheet name="Extra Sheet for Math" sheetId="3" r:id="rId2"/>
+    <sheet name="Literature PURE All µM" sheetId="4" r:id="rId3"/>
+    <sheet name="tRNA Abundances E. coli" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -126,8 +128,260 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="J7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Liposome Display Paper, so formula is optimized for this purpose</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+See next tab for predicted abundances
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K36" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Not in PURE solutions A or B itself, but in liposome outer solution</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D75" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Somewhat unclear via wording of the paper</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="E4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Liposome Display Paper, so formula is optimized for this purpose</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+See next tab for predicted abundances
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Not in PURE solutions A or B itself, but in liposome outer solution</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C72" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Somewhat unclear via wording of the paper</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="B20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+there is another ile in here source: conary table</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+there is another leu here</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="136">
   <si>
     <t>PURE Component</t>
   </si>
@@ -526,13 +780,22 @@
   </si>
   <si>
     <t>–</t>
+  </si>
+  <si>
+    <t>kDa</t>
+  </si>
+  <si>
+    <t># Molecules / L</t>
+  </si>
+  <si>
+    <t>2.16 µg/µL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -582,6 +845,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -618,14 +891,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -635,13 +919,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3693,11 +3979,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1135585760"/>
-        <c:axId val="1137426896"/>
+        <c:axId val="1185822176"/>
+        <c:axId val="1185824368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1135585760"/>
+        <c:axId val="1185822176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3820,7 +4106,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1137426896"/>
+        <c:crossAx val="1185824368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3828,7 +4114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1137426896"/>
+        <c:axId val="1185824368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3946,7 +4232,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1135585760"/>
+        <c:crossAx val="1185822176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4851,8 +5137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="G24:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4863,20 +5149,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -5871,7 +6157,7 @@
         <f>16*2.3/30</f>
         <v>1.2266666666666666</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="E59" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5889,7 +6175,7 @@
         <f>14*2.3/30</f>
         <v>1.0733333333333333</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E60" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5907,7 +6193,7 @@
         <f>100*2.3/30</f>
         <v>7.6666666666666661</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="E61" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5925,7 +6211,7 @@
         <f>43*2.3/30</f>
         <v>3.2966666666666664</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E62" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5943,7 +6229,7 @@
         <f>0.64*2.3/30</f>
         <v>4.9066666666666668E-2</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E63" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5961,7 +6247,7 @@
         <f>2.2*2.3/30</f>
         <v>0.16866666666666666</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E64" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5979,7 +6265,7 @@
         <f>51*2.3/30</f>
         <v>3.9099999999999997</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="E65" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5997,7 +6283,7 @@
         <f>3.2*2.3/30</f>
         <v>0.24533333333333332</v>
       </c>
-      <c r="E66" s="7" t="s">
+      <c r="E66" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -6015,7 +6301,7 @@
         <f>18*2.3/30</f>
         <v>1.38</v>
       </c>
-      <c r="E67" s="7" t="s">
+      <c r="E67" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -6033,7 +6319,7 @@
         <f>0.21*2.3/30</f>
         <v>1.6099999999999996E-2</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E68" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -6051,7 +6337,7 @@
         <f>0.53*2.3/30</f>
         <v>4.0633333333333327E-2</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E69" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -6121,11 +6407,3198 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C6:M82"/>
+  <sheetViews>
+    <sheetView topLeftCell="B55" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41:J77"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="D6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="D7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="3"/>
+      <c r="J7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <f>D9*1000</f>
+        <v>100</v>
+      </c>
+      <c r="J9">
+        <v>0.3</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9">
+        <f>1000*J9</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ref="H10:H28" si="0">D10*1000</f>
+        <v>100</v>
+      </c>
+      <c r="J10">
+        <v>0.3</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:L28" si="1">1000*J10</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>0.1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J11">
+        <v>0.3</v>
+      </c>
+      <c r="K11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>0.1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <v>0.3</v>
+      </c>
+      <c r="K12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J13">
+        <v>0.3</v>
+      </c>
+      <c r="K13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J14">
+        <v>0.3</v>
+      </c>
+      <c r="K14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>0.1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J15">
+        <v>0.3</v>
+      </c>
+      <c r="K15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>0.1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J16">
+        <v>0.3</v>
+      </c>
+      <c r="K16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J17">
+        <v>0.3</v>
+      </c>
+      <c r="K17" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>0.1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J18">
+        <v>0.3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>0.1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J19">
+        <v>0.3</v>
+      </c>
+      <c r="K19" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>0.1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J20">
+        <v>0.3</v>
+      </c>
+      <c r="K20" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>0.1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J21">
+        <v>0.3</v>
+      </c>
+      <c r="K21" t="s">
+        <v>25</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22">
+        <v>0.1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J22">
+        <v>0.3</v>
+      </c>
+      <c r="K22" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23">
+        <v>0.1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J23">
+        <v>0.3</v>
+      </c>
+      <c r="K23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>0.1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J24">
+        <v>0.3</v>
+      </c>
+      <c r="K24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25">
+        <v>0.1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J25">
+        <v>0.3</v>
+      </c>
+      <c r="K25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26">
+        <v>0.1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J26">
+        <v>0.3</v>
+      </c>
+      <c r="K26" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="M26" s="10"/>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27">
+        <v>0.1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J27">
+        <v>0.3</v>
+      </c>
+      <c r="K27" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="M27" s="10"/>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <v>0.1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J28">
+        <v>0.3</v>
+      </c>
+      <c r="K28" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="M28" s="10"/>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <f>108/2</f>
+        <v>54</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>135</v>
+      </c>
+      <c r="G29">
+        <v>84.58</v>
+      </c>
+      <c r="H29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J29">
+        <v>24</v>
+      </c>
+      <c r="K29" t="s">
+        <v>78</v>
+      </c>
+      <c r="L29">
+        <v>939.79</v>
+      </c>
+      <c r="M29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30">
+        <f>D30*1000</f>
+        <v>2000</v>
+      </c>
+      <c r="J30">
+        <f>7.5/2</f>
+        <v>3.75</v>
+      </c>
+      <c r="K30" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30">
+        <f>J30*1000</f>
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ref="H31:H36" si="2">D31*1000</f>
+        <v>2000</v>
+      </c>
+      <c r="J31">
+        <v>2.5</v>
+      </c>
+      <c r="K31" t="s">
+        <v>25</v>
+      </c>
+      <c r="L31">
+        <f t="shared" ref="L31:L34" si="3">J31*1000</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="J32">
+        <v>1.25</v>
+      </c>
+      <c r="K32" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="3"/>
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="J33">
+        <v>1.25</v>
+      </c>
+      <c r="K33" t="s">
+        <v>25</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="3"/>
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34">
+        <v>20</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="2"/>
+        <v>20000</v>
+      </c>
+      <c r="J34">
+        <v>25</v>
+      </c>
+      <c r="K34" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="3"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35">
+        <v>473.44600000000003</v>
+      </c>
+      <c r="G35">
+        <f>D35/(F35*1000)</f>
+        <v>2.1121732995948853E-5</v>
+      </c>
+      <c r="H35">
+        <f>G35*1000</f>
+        <v>2.1121732995948852E-2</v>
+      </c>
+      <c r="J35">
+        <v>10</v>
+      </c>
+      <c r="K35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36">
+        <v>50</v>
+      </c>
+      <c r="E36" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36">
+        <f>D36*1000</f>
+        <v>50000</v>
+      </c>
+      <c r="J36" t="s">
+        <v>132</v>
+      </c>
+      <c r="K36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37">
+        <v>100</v>
+      </c>
+      <c r="E37" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37">
+        <f t="shared" ref="H37:H40" si="4">D37*1000</f>
+        <v>100000</v>
+      </c>
+      <c r="J37">
+        <f>560/2</f>
+        <v>280</v>
+      </c>
+      <c r="K37" t="s">
+        <v>25</v>
+      </c>
+      <c r="L37">
+        <f>J37*1000</f>
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="4"/>
+        <v>13000</v>
+      </c>
+      <c r="J38">
+        <f>49/2</f>
+        <v>24.5</v>
+      </c>
+      <c r="K38" t="s">
+        <v>25</v>
+      </c>
+      <c r="L38">
+        <f t="shared" ref="L38:L40" si="5">J38*1000</f>
+        <v>24500</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="J39">
+        <v>1.5</v>
+      </c>
+      <c r="K39" t="s">
+        <v>25</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="5"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="J40">
+        <v>1.5</v>
+      </c>
+      <c r="K40" t="s">
+        <v>25</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="5"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41">
+        <v>69</v>
+      </c>
+      <c r="E41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="10">
+        <v>96.36</v>
+      </c>
+      <c r="G41">
+        <f>D41*6.0221366516752*10^20/(F41*1000)</f>
+        <v>4.3122398190700371E+17</v>
+      </c>
+      <c r="H41">
+        <f>G41*10^6/(6.0221366516752*10^23)</f>
+        <v>0.71606475716064766</v>
+      </c>
+      <c r="J41">
+        <f>9.5*2.3/30</f>
+        <v>0.72833333333333328</v>
+      </c>
+      <c r="K41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" s="10">
+        <v>63.47</v>
+      </c>
+      <c r="G42">
+        <f t="shared" ref="G42:G77" si="6">D42*6.0221366516752*10^20/(F42*1000)</f>
+        <v>1.8976324725619032E+16</v>
+      </c>
+      <c r="H42">
+        <f t="shared" ref="H42:H77" si="7">G42*10^6/(6.0221366516752*10^23)</f>
+        <v>3.1510950055144163E-2</v>
+      </c>
+      <c r="J42">
+        <f>0.4*2.3/30</f>
+        <v>3.0666666666666665E-2</v>
+      </c>
+      <c r="K42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43">
+        <v>22</v>
+      </c>
+      <c r="E43" t="s">
+        <v>34</v>
+      </c>
+      <c r="F43" s="10">
+        <v>51.26</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="6"/>
+        <v>2.5846080050108154E+17</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="7"/>
+        <v>0.42918454935622319</v>
+      </c>
+      <c r="J43">
+        <f>5.5*2.3/30</f>
+        <v>0.42166666666666663</v>
+      </c>
+      <c r="K43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="10">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="6"/>
+        <v>7.4232809265641904E+16</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="7"/>
+        <v>0.12326656394453005</v>
+      </c>
+      <c r="J44">
+        <f>1.6*2.3/30</f>
+        <v>0.12266666666666666</v>
+      </c>
+      <c r="K44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45">
+        <v>1.2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" s="10">
+        <v>50.71</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="6"/>
+        <v>1.4250767071603706E+16</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="7"/>
+        <v>2.3663971603234076E-2</v>
+      </c>
+      <c r="J45">
+        <f>0.31*2.3/30</f>
+        <v>2.3766666666666665E-2</v>
+      </c>
+      <c r="K45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46">
+        <v>3.8</v>
+      </c>
+      <c r="E46" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" s="10">
+        <v>60.94</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="6"/>
+        <v>3.7551885914613976E+16</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="7"/>
+        <v>6.2356416147029865E-2</v>
+      </c>
+      <c r="J46">
+        <f>0.78*2.3/30</f>
+        <v>5.9799999999999992E-2</v>
+      </c>
+      <c r="K46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47">
+        <v>12.6</v>
+      </c>
+      <c r="E47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="10">
+        <v>51.81</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="6"/>
+        <v>1.4645613165625846E+17</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="7"/>
+        <v>0.24319629415170818</v>
+      </c>
+      <c r="J47">
+        <f>3*2.3/30</f>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="K47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48">
+        <v>9.6</v>
+      </c>
+      <c r="E48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48">
+        <f>75.79+33.33</f>
+        <v>109.12</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="6"/>
+        <v>5.2980674354913776E+16</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="7"/>
+        <v>8.797653958944282E-2</v>
+      </c>
+      <c r="J48">
+        <f>1.1*2.3/30</f>
+        <v>8.433333333333333E-2</v>
+      </c>
+      <c r="K48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49">
+        <v>0.8</v>
+      </c>
+      <c r="E49" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" s="10">
+        <v>46.64</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="6"/>
+        <v>1.032956544026621E+16</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="7"/>
+        <v>1.7152658662092625E-2</v>
+      </c>
+      <c r="J49">
+        <f>1.1*2.3/30</f>
+        <v>8.433333333333333E-2</v>
+      </c>
+      <c r="K49" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50">
+        <v>40</v>
+      </c>
+      <c r="E50" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" s="10">
+        <v>103.18</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="6"/>
+        <v>2.3346139374588877E+17</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="7"/>
+        <v>0.38767202946307433</v>
+      </c>
+      <c r="J50">
+        <f>4.8*2.3/30</f>
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="K50" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+      <c r="E51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" s="10">
+        <v>94.6</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="6"/>
+        <v>2.5463579922516704E+16</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="7"/>
+        <v>4.22832980972516E-2</v>
+      </c>
+      <c r="J51">
+        <f>0.53*2.3/30</f>
+        <v>4.0633333333333327E-2</v>
+      </c>
+      <c r="K51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52">
+        <v>6.4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>34</v>
+      </c>
+      <c r="F52" s="10">
+        <v>55.55</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="6"/>
+        <v>6.9381952422540568E+16</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="7"/>
+        <v>0.11521152115211523</v>
+      </c>
+      <c r="J52">
+        <f>1.5*2.3/30</f>
+        <v>0.11499999999999999</v>
+      </c>
+      <c r="K52" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53">
+        <v>2.1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>34</v>
+      </c>
+      <c r="F53" s="10">
+        <v>74.47</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="6"/>
+        <v>1.69819886780152E+16</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="7"/>
+        <v>2.819927487578891E-2</v>
+      </c>
+      <c r="J53">
+        <f>1.4*2.3/30</f>
+        <v>0.10733333333333332</v>
+      </c>
+      <c r="K53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>53</v>
+      </c>
+      <c r="D54">
+        <v>17</v>
+      </c>
+      <c r="E54" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54">
+        <f>35.97+87.45</f>
+        <v>123.42</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="6"/>
+        <v>8.29495406566832E+16</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="7"/>
+        <v>0.13774104683195595</v>
+      </c>
+      <c r="J54">
+        <f>1.7*2.3/30</f>
+        <v>0.13033333333333333</v>
+      </c>
+      <c r="K54" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55">
+        <v>10</v>
+      </c>
+      <c r="E55" t="s">
+        <v>34</v>
+      </c>
+      <c r="F55" s="10">
+        <v>62.92</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="6"/>
+        <v>9.5711008450019072E+16</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="7"/>
+        <v>0.15893197711379531</v>
+      </c>
+      <c r="J55">
+        <f>2.2*2.3/30</f>
+        <v>0.16866666666666666</v>
+      </c>
+      <c r="K55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56">
+        <v>1.9</v>
+      </c>
+      <c r="E56" t="s">
+        <v>34</v>
+      </c>
+      <c r="F56" s="10">
+        <v>47.3</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="6"/>
+        <v>2.4190400926390864E+16</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="7"/>
+        <v>4.0169133192389003E-2</v>
+      </c>
+      <c r="J56">
+        <f>1*2.3/30</f>
+        <v>7.6666666666666661E-2</v>
+      </c>
+      <c r="K56" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57">
+        <v>6.3</v>
+      </c>
+      <c r="E57" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" s="10">
+        <v>70.62</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="6"/>
+        <v>5.3723394088861168E+16</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="7"/>
+        <v>8.9209855564995763E-2</v>
+      </c>
+      <c r="J57">
+        <f>1.1*2.3/30</f>
+        <v>8.433333333333333E-2</v>
+      </c>
+      <c r="K57" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
+        <v>57</v>
+      </c>
+      <c r="D58">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E58" t="s">
+        <v>34</v>
+      </c>
+      <c r="F58" s="10">
+        <v>36.74</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="6"/>
+        <v>1.8030349256512576E+16</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="7"/>
+        <v>2.9940119760479045E-2</v>
+      </c>
+      <c r="J58">
+        <f>0.37*2.3/30</f>
+        <v>2.8366666666666665E-2</v>
+      </c>
+      <c r="K58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
+        <v>58</v>
+      </c>
+      <c r="D59">
+        <v>0.6</v>
+      </c>
+      <c r="E59" t="s">
+        <v>34</v>
+      </c>
+      <c r="F59" s="10">
+        <v>46.64</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="6"/>
+        <v>7747174080199656</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="7"/>
+        <v>1.2864493996569469E-2</v>
+      </c>
+      <c r="J59">
+        <f>2*2.3/30</f>
+        <v>0.15333333333333332</v>
+      </c>
+      <c r="K59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60">
+        <v>1.8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>34</v>
+      </c>
+      <c r="F60" s="10">
+        <v>104.61</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="6"/>
+        <v>1.0362150820203958E+16</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="7"/>
+        <v>1.7206767995411532E-2</v>
+      </c>
+      <c r="J60">
+        <f>0.22*2.3/30</f>
+        <v>1.6866666666666665E-2</v>
+      </c>
+      <c r="K60" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>60</v>
+      </c>
+      <c r="D61">
+        <v>20</v>
+      </c>
+      <c r="E61" t="s">
+        <v>34</v>
+      </c>
+      <c r="F61" s="10">
+        <v>34.65</v>
+      </c>
+      <c r="G61">
+        <f>D61*6.0221366516752*10^20/(F61*1000)</f>
+        <v>3.4759807513276768E+17</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="7"/>
+        <v>0.57720057720057727</v>
+      </c>
+      <c r="J61">
+        <f>7.7*2.3/30</f>
+        <v>0.59033333333333327</v>
+      </c>
+      <c r="K61" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62">
+        <v>10</v>
+      </c>
+      <c r="E62" t="s">
+        <v>34</v>
+      </c>
+      <c r="F62" s="10">
+        <v>7.92</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="6"/>
+        <v>7.6037078935292928E+17</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="7"/>
+        <v>1.2626262626262628</v>
+      </c>
+      <c r="J62">
+        <f>320*2.3/30</f>
+        <v>24.533333333333335</v>
+      </c>
+      <c r="K62" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
+        <v>62</v>
+      </c>
+      <c r="D63">
+        <v>40</v>
+      </c>
+      <c r="E63" t="s">
+        <v>34</v>
+      </c>
+      <c r="F63" s="10">
+        <v>97.9</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="6"/>
+        <v>2.4605257003780186E+17</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="7"/>
+        <v>0.4085801838610828</v>
+      </c>
+      <c r="J63">
+        <f>13*2.3/30</f>
+        <v>0.99666666666666659</v>
+      </c>
+      <c r="K63" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>63</v>
+      </c>
+      <c r="D64">
+        <v>10</v>
+      </c>
+      <c r="E64" t="s">
+        <v>34</v>
+      </c>
+      <c r="F64" s="10">
+        <v>19.8</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="6"/>
+        <v>3.0414831574117171E+17</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="7"/>
+        <v>0.50505050505050508</v>
+      </c>
+      <c r="J64">
+        <f>16*2.3/30</f>
+        <v>1.2266666666666666</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65">
+        <v>50</v>
+      </c>
+      <c r="E65" t="s">
+        <v>34</v>
+      </c>
+      <c r="F65" s="10">
+        <v>77.44</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="6"/>
+        <v>3.8882597182820243E+17</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="7"/>
+        <v>0.64566115702479332</v>
+      </c>
+      <c r="J65">
+        <f>14*2.3/30</f>
+        <v>1.0733333333333333</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>65</v>
+      </c>
+      <c r="D66">
+        <v>100</v>
+      </c>
+      <c r="E66" t="s">
+        <v>34</v>
+      </c>
+      <c r="F66" s="10">
+        <v>43.34</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="6"/>
+        <v>1.3895100719139822E+18</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="7"/>
+        <v>2.3073373327180429</v>
+      </c>
+      <c r="J66">
+        <f>100*2.3/30</f>
+        <v>7.6666666666666661</v>
+      </c>
+      <c r="K66" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67">
+        <v>50</v>
+      </c>
+      <c r="E67" t="s">
+        <v>34</v>
+      </c>
+      <c r="F67" s="10">
+        <v>31.13</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="6"/>
+        <v>9.6725612779877914E+17</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="7"/>
+        <v>1.6061676839061996</v>
+      </c>
+      <c r="J67">
+        <f>43*2.3/30</f>
+        <v>3.2966666666666664</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
+        <v>67</v>
+      </c>
+      <c r="D68">
+        <v>10</v>
+      </c>
+      <c r="E68" t="s">
+        <v>34</v>
+      </c>
+      <c r="F68" s="11">
+        <v>39.6</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="6"/>
+        <v>1.5207415787058586E+17</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="7"/>
+        <v>0.25252525252525254</v>
+      </c>
+      <c r="J68">
+        <f>0.64*2.3/30</f>
+        <v>4.9066666666666668E-2</v>
+      </c>
+      <c r="K68" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="69" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>68</v>
+      </c>
+      <c r="D69">
+        <v>10</v>
+      </c>
+      <c r="E69" t="s">
+        <v>34</v>
+      </c>
+      <c r="F69" s="11">
+        <v>58.19</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="6"/>
+        <v>1.0349092029000173E+17</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="7"/>
+        <v>0.1718508334765424</v>
+      </c>
+      <c r="J69">
+        <f>2.2*2.3/30</f>
+        <v>0.16866666666666666</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>69</v>
+      </c>
+      <c r="D70">
+        <v>10</v>
+      </c>
+      <c r="E70" t="s">
+        <v>34</v>
+      </c>
+      <c r="F70" s="10">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="6"/>
+        <v>2.9592809099141037E+17</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="7"/>
+        <v>0.49140049140049158</v>
+      </c>
+      <c r="J70">
+        <f>51*2.3/30</f>
+        <v>3.9099999999999997</v>
+      </c>
+      <c r="K70" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
+        <v>70</v>
+      </c>
+      <c r="D71">
+        <v>4</v>
+      </c>
+      <c r="E71" t="s">
+        <v>34</v>
+      </c>
+      <c r="F71" s="10">
+        <v>43.112000000000002</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="6"/>
+        <v>5.587434265796252E+16</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="7"/>
+        <v>9.2781592132120991E-2</v>
+      </c>
+      <c r="J71">
+        <f>3.2*2.3/30</f>
+        <v>0.24533333333333332</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="72" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>71</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72" t="s">
+        <v>34</v>
+      </c>
+      <c r="F72" s="10">
+        <v>23.54</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="6"/>
+        <v>7.674770584123024E+16</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="7"/>
+        <v>0.12744265080713679</v>
+      </c>
+      <c r="J72">
+        <f>18*2.3/30</f>
+        <v>1.38</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D73">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E73" t="s">
+        <v>34</v>
+      </c>
+      <c r="F73" s="10">
+        <v>15.73</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="6"/>
+        <v>4.21128437180084E+16</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="7"/>
+        <v>6.9930069930069963E-2</v>
+      </c>
+      <c r="J73">
+        <f>0.21*2.3/30</f>
+        <v>1.6099999999999996E-2</v>
+      </c>
+      <c r="K73" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
+        <v>73</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
+        <v>34</v>
+      </c>
+      <c r="F74" s="10">
+        <v>19.36</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="6"/>
+        <v>3.11060777462562E+16</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="7"/>
+        <v>5.1652892561983479E-2</v>
+      </c>
+      <c r="J74">
+        <f>0.53*2.3/30</f>
+        <v>4.0633333333333327E-2</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>74</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>34</v>
+      </c>
+      <c r="F75" s="10">
+        <v>99</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="6"/>
+        <v>6082966314823435</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="7"/>
+        <v>1.0101010101010104E-2</v>
+      </c>
+      <c r="J75">
+        <f>1.3/2</f>
+        <v>0.65</v>
+      </c>
+      <c r="K75" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="76" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
+        <v>75</v>
+      </c>
+      <c r="D76">
+        <v>1.2</v>
+      </c>
+      <c r="E76" t="s">
+        <v>76</v>
+      </c>
+      <c r="J76">
+        <f>39/2</f>
+        <v>19.5</v>
+      </c>
+      <c r="K76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>131</v>
+      </c>
+      <c r="D77" t="s">
+        <v>132</v>
+      </c>
+      <c r="E77" t="s">
+        <v>132</v>
+      </c>
+      <c r="F77" s="10">
+        <v>44</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <f>2.2*2.3/30</f>
+        <v>0.16866666666666666</v>
+      </c>
+      <c r="K77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="J7:K7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6">
+        <v>300</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7">
+        <v>300</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8">
+        <v>300</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>300</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10">
+        <v>300</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11">
+        <v>300</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12">
+        <v>300</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13">
+        <v>300</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14">
+        <v>300</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15">
+        <v>300</v>
+      </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16">
+        <v>300</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17">
+        <v>300</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18">
+        <v>300</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+      <c r="D19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19">
+        <v>300</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20">
+        <v>300</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21">
+        <v>300</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>100</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22">
+        <v>300</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>100</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23">
+        <v>300</v>
+      </c>
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24">
+        <v>300</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>100</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25">
+        <v>300</v>
+      </c>
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>84.58</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26">
+        <v>939.79</v>
+      </c>
+      <c r="F26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>2000</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27">
+        <v>3750</v>
+      </c>
+      <c r="F27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28">
+        <v>2000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28">
+        <v>2500</v>
+      </c>
+      <c r="F28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>1000</v>
+      </c>
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29">
+        <v>1250</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30">
+        <v>1000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30">
+        <v>1250</v>
+      </c>
+      <c r="F30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>20000</v>
+      </c>
+      <c r="D31" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31">
+        <v>25000</v>
+      </c>
+      <c r="F31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32">
+        <v>2.1121732995948852E-2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32">
+        <v>2.1121732995948852E-2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33">
+        <v>50000</v>
+      </c>
+      <c r="D33" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" t="s">
+        <v>132</v>
+      </c>
+      <c r="F33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34">
+        <v>100000</v>
+      </c>
+      <c r="D34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34">
+        <v>280000</v>
+      </c>
+      <c r="F34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35">
+        <v>13000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35">
+        <v>24500</v>
+      </c>
+      <c r="F35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36">
+        <v>2000</v>
+      </c>
+      <c r="D36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36">
+        <v>1500</v>
+      </c>
+      <c r="F36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37">
+        <v>1000</v>
+      </c>
+      <c r="D37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37">
+        <v>1500</v>
+      </c>
+      <c r="F37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38">
+        <v>0.71606475716064766</v>
+      </c>
+      <c r="D38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38">
+        <v>0.72833333333333328</v>
+      </c>
+      <c r="F38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39">
+        <v>3.1510950055144163E-2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39">
+        <v>3.0666666666666665E-2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40">
+        <v>0.42918454935622319</v>
+      </c>
+      <c r="D40" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40">
+        <v>0.42166666666666663</v>
+      </c>
+      <c r="F40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41">
+        <v>0.12326656394453005</v>
+      </c>
+      <c r="D41" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41">
+        <v>0.12266666666666666</v>
+      </c>
+      <c r="F41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42">
+        <v>2.3663971603234076E-2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42">
+        <v>2.3766666666666665E-2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43">
+        <v>6.2356416147029865E-2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>76</v>
+      </c>
+      <c r="E43">
+        <v>5.9799999999999992E-2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44">
+        <v>0.24319629415170818</v>
+      </c>
+      <c r="D44" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44">
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="F44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45">
+        <v>8.797653958944282E-2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45">
+        <v>8.433333333333333E-2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46">
+        <v>1.7152658662092625E-2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46">
+        <v>8.433333333333333E-2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47">
+        <v>0.38767202946307433</v>
+      </c>
+      <c r="D47" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="F47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48">
+        <v>4.22832980972516E-2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48">
+        <v>4.0633333333333327E-2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49">
+        <v>0.11521152115211523</v>
+      </c>
+      <c r="D49" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49">
+        <v>0.11499999999999999</v>
+      </c>
+      <c r="F49" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50">
+        <v>2.819927487578891E-2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50">
+        <v>0.10733333333333332</v>
+      </c>
+      <c r="F50" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51">
+        <v>0.13774104683195595</v>
+      </c>
+      <c r="D51" t="s">
+        <v>76</v>
+      </c>
+      <c r="E51">
+        <v>0.13033333333333333</v>
+      </c>
+      <c r="F51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52">
+        <v>0.15893197711379531</v>
+      </c>
+      <c r="D52" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52">
+        <v>0.16866666666666666</v>
+      </c>
+      <c r="F52" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53">
+        <v>4.0169133192389003E-2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>76</v>
+      </c>
+      <c r="E53">
+        <v>7.6666666666666661E-2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54">
+        <v>8.9209855564995763E-2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>76</v>
+      </c>
+      <c r="E54">
+        <v>8.433333333333333E-2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>57</v>
+      </c>
+      <c r="C55">
+        <v>2.9940119760479045E-2</v>
+      </c>
+      <c r="D55" t="s">
+        <v>76</v>
+      </c>
+      <c r="E55">
+        <v>2.8366666666666665E-2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56">
+        <v>1.2864493996569469E-2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>76</v>
+      </c>
+      <c r="E56">
+        <v>0.15333333333333332</v>
+      </c>
+      <c r="F56" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57">
+        <v>1.7206767995411532E-2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57">
+        <v>1.6866666666666665E-2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58">
+        <v>0.57720057720057727</v>
+      </c>
+      <c r="D58" t="s">
+        <v>76</v>
+      </c>
+      <c r="E58">
+        <v>0.59033333333333327</v>
+      </c>
+      <c r="F58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59">
+        <v>1.2626262626262628</v>
+      </c>
+      <c r="D59" t="s">
+        <v>76</v>
+      </c>
+      <c r="E59">
+        <v>24.533333333333335</v>
+      </c>
+      <c r="F59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60">
+        <v>0.4085801838610828</v>
+      </c>
+      <c r="D60" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60">
+        <v>0.99666666666666659</v>
+      </c>
+      <c r="F60" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61">
+        <v>0.50505050505050508</v>
+      </c>
+      <c r="D61" t="s">
+        <v>76</v>
+      </c>
+      <c r="E61">
+        <v>1.2266666666666666</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62">
+        <v>0.64566115702479332</v>
+      </c>
+      <c r="D62" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62">
+        <v>1.0733333333333333</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63">
+        <v>2.3073373327180429</v>
+      </c>
+      <c r="D63" t="s">
+        <v>76</v>
+      </c>
+      <c r="E63">
+        <v>7.6666666666666661</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64">
+        <v>1.6061676839061996</v>
+      </c>
+      <c r="D64" t="s">
+        <v>76</v>
+      </c>
+      <c r="E64">
+        <v>3.2966666666666664</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65">
+        <v>0.25252525252525254</v>
+      </c>
+      <c r="D65" t="s">
+        <v>76</v>
+      </c>
+      <c r="E65">
+        <v>4.9066666666666668E-2</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>68</v>
+      </c>
+      <c r="C66">
+        <v>0.1718508334765424</v>
+      </c>
+      <c r="D66" t="s">
+        <v>76</v>
+      </c>
+      <c r="E66">
+        <v>0.16866666666666666</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>69</v>
+      </c>
+      <c r="C67">
+        <v>0.49140049140049158</v>
+      </c>
+      <c r="D67" t="s">
+        <v>76</v>
+      </c>
+      <c r="E67">
+        <v>3.9099999999999997</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68">
+        <v>9.2781592132120991E-2</v>
+      </c>
+      <c r="D68" t="s">
+        <v>76</v>
+      </c>
+      <c r="E68">
+        <v>0.24533333333333332</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>71</v>
+      </c>
+      <c r="C69">
+        <v>0.12744265080713679</v>
+      </c>
+      <c r="D69" t="s">
+        <v>76</v>
+      </c>
+      <c r="E69">
+        <v>1.38</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>72</v>
+      </c>
+      <c r="C70">
+        <v>6.9930069930069963E-2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>76</v>
+      </c>
+      <c r="E70">
+        <v>1.6099999999999996E-2</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>73</v>
+      </c>
+      <c r="C71">
+        <v>5.1652892561983479E-2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>76</v>
+      </c>
+      <c r="E71">
+        <v>4.0633333333333327E-2</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72">
+        <v>1.0101010101010104E-2</v>
+      </c>
+      <c r="D72" t="s">
+        <v>76</v>
+      </c>
+      <c r="E72">
+        <v>0.65</v>
+      </c>
+      <c r="F72" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>75</v>
+      </c>
+      <c r="C73">
+        <v>1.2</v>
+      </c>
+      <c r="D73" t="s">
+        <v>76</v>
+      </c>
+      <c r="E73">
+        <v>19.5</v>
+      </c>
+      <c r="F73" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>131</v>
+      </c>
+      <c r="C74" t="s">
+        <v>132</v>
+      </c>
+      <c r="D74" t="s">
+        <v>132</v>
+      </c>
+      <c r="E74">
+        <v>0.16866666666666666</v>
+      </c>
+      <c r="F74" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6143,22 +9616,22 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>0.4</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.7</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>1.07</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>1.6</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>2.5</v>
       </c>
     </row>
@@ -7075,7 +10548,7 @@
         <v>216.90999999999994</v>
       </c>
       <c r="E51" s="1">
-        <f t="shared" ref="D51:G51" si="0">SUM(E5:E48)</f>
+        <f t="shared" ref="E51:G51" si="0">SUM(E5:E48)</f>
         <v>237.57999999999993</v>
       </c>
       <c r="F51" s="1">
@@ -7093,22 +10566,22 @@
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C54" s="6">
+      <c r="C54" s="5">
         <v>0.4</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="5">
         <v>0.7</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="5">
         <v>1.07</v>
       </c>
-      <c r="F54" s="6">
+      <c r="F54" s="5">
         <v>1.6</v>
       </c>
-      <c r="G54" s="6">
+      <c r="G54" s="5">
         <v>2.5</v>
       </c>
     </row>
@@ -7162,7 +10635,7 @@
         <v>85</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:G99" si="1">C6*100/$C$51</f>
+        <f t="shared" ref="C57:C99" si="1">C6*100/$C$51</f>
         <v>0.95945679984255061</v>
       </c>
       <c r="D57">
@@ -8235,5 +11708,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated re: Eric's comments
</commit_message>
<xml_diff>
--- a/modeling/PURE Formulations.xlsx
+++ b/modeling/PURE Formulations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="21700" windowHeight="16120" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1180" yWindow="560" windowWidth="21700" windowHeight="16120" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Literature PURE" sheetId="1" r:id="rId1"/>
@@ -300,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C72" authorId="0">
+    <comment ref="C73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -891,8 +891,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -923,11 +925,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6410,7 +6414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:M82"/>
   <sheetViews>
-    <sheetView topLeftCell="B55" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J41" sqref="J41:J77"/>
     </sheetView>
   </sheetViews>
@@ -8366,7 +8370,7 @@
   <dimension ref="B3:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8423,7 +8427,7 @@
         <v>300</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -8440,7 +8444,7 @@
         <v>300</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
@@ -8457,7 +8461,7 @@
         <v>300</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
@@ -8474,7 +8478,7 @@
         <v>300</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
@@ -8491,7 +8495,7 @@
         <v>300</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
@@ -8508,7 +8512,7 @@
         <v>300</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
@@ -8525,7 +8529,7 @@
         <v>300</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
@@ -8542,7 +8546,7 @@
         <v>300</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
@@ -8559,7 +8563,7 @@
         <v>300</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
@@ -8576,7 +8580,7 @@
         <v>300</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
@@ -8593,7 +8597,7 @@
         <v>300</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -8610,7 +8614,7 @@
         <v>300</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
@@ -8627,7 +8631,7 @@
         <v>300</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
@@ -8644,7 +8648,7 @@
         <v>300</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
@@ -8661,7 +8665,7 @@
         <v>300</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
@@ -8678,7 +8682,7 @@
         <v>300</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
@@ -8695,7 +8699,7 @@
         <v>300</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
@@ -8712,7 +8716,7 @@
         <v>300</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
@@ -8729,7 +8733,7 @@
         <v>300</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
@@ -8746,7 +8750,7 @@
         <v>300</v>
       </c>
       <c r="F25" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
@@ -8780,7 +8784,7 @@
         <v>3750</v>
       </c>
       <c r="F27" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
@@ -8797,7 +8801,7 @@
         <v>2500</v>
       </c>
       <c r="F28" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
@@ -8814,7 +8818,7 @@
         <v>1250</v>
       </c>
       <c r="F29" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
@@ -8831,7 +8835,7 @@
         <v>1250</v>
       </c>
       <c r="F30" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
@@ -8848,7 +8852,7 @@
         <v>25000</v>
       </c>
       <c r="F31" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
@@ -8882,7 +8886,7 @@
         <v>132</v>
       </c>
       <c r="F33" t="s">
-        <v>132</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
@@ -8899,7 +8903,7 @@
         <v>280000</v>
       </c>
       <c r="F34" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
@@ -8916,7 +8920,7 @@
         <v>24500</v>
       </c>
       <c r="F35" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
@@ -8933,7 +8937,7 @@
         <v>1500</v>
       </c>
       <c r="F36" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
@@ -8950,7 +8954,7 @@
         <v>1500</v>
       </c>
       <c r="F37" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
@@ -9357,7 +9361,7 @@
       <c r="E61">
         <v>1.2266666666666666</v>
       </c>
-      <c r="F61" s="6" t="s">
+      <c r="F61" t="s">
         <v>76</v>
       </c>
     </row>
@@ -9374,7 +9378,7 @@
       <c r="E62">
         <v>1.0733333333333333</v>
       </c>
-      <c r="F62" s="6" t="s">
+      <c r="F62" t="s">
         <v>76</v>
       </c>
     </row>
@@ -9391,7 +9395,7 @@
       <c r="E63">
         <v>7.6666666666666661</v>
       </c>
-      <c r="F63" s="6" t="s">
+      <c r="F63" t="s">
         <v>76</v>
       </c>
     </row>
@@ -9408,7 +9412,7 @@
       <c r="E64">
         <v>3.2966666666666664</v>
       </c>
-      <c r="F64" s="6" t="s">
+      <c r="F64" t="s">
         <v>76</v>
       </c>
     </row>
@@ -9425,124 +9429,124 @@
       <c r="E65">
         <v>4.9066666666666668E-2</v>
       </c>
-      <c r="F65" s="6" t="s">
+      <c r="F65" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>68</v>
-      </c>
-      <c r="C66">
-        <v>0.1718508334765424</v>
+        <v>131</v>
+      </c>
+      <c r="C66" t="s">
+        <v>132</v>
       </c>
       <c r="D66" t="s">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="E66">
         <v>0.16866666666666666</v>
       </c>
-      <c r="F66" s="6" t="s">
+      <c r="F66" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C67">
-        <v>0.49140049140049158</v>
+        <v>0.1718508334765424</v>
       </c>
       <c r="D67" t="s">
         <v>76</v>
       </c>
       <c r="E67">
-        <v>3.9099999999999997</v>
-      </c>
-      <c r="F67" s="6" t="s">
+        <v>0.16866666666666666</v>
+      </c>
+      <c r="F67" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C68">
-        <v>9.2781592132120991E-2</v>
+        <v>0.49140049140049158</v>
       </c>
       <c r="D68" t="s">
         <v>76</v>
       </c>
       <c r="E68">
-        <v>0.24533333333333332</v>
-      </c>
-      <c r="F68" s="6" t="s">
+        <v>3.9099999999999997</v>
+      </c>
+      <c r="F68" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C69">
-        <v>0.12744265080713679</v>
+        <v>9.2781592132120991E-2</v>
       </c>
       <c r="D69" t="s">
         <v>76</v>
       </c>
       <c r="E69">
-        <v>1.38</v>
-      </c>
-      <c r="F69" s="6" t="s">
+        <v>0.24533333333333332</v>
+      </c>
+      <c r="F69" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C70">
-        <v>6.9930069930069963E-2</v>
+        <v>0.12744265080713679</v>
       </c>
       <c r="D70" t="s">
         <v>76</v>
       </c>
       <c r="E70">
-        <v>1.6099999999999996E-2</v>
-      </c>
-      <c r="F70" s="6" t="s">
+        <v>1.38</v>
+      </c>
+      <c r="F70" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C71">
-        <v>5.1652892561983479E-2</v>
+        <v>6.9930069930069963E-2</v>
       </c>
       <c r="D71" t="s">
         <v>76</v>
       </c>
       <c r="E71">
-        <v>4.0633333333333327E-2</v>
-      </c>
-      <c r="F71" s="6" t="s">
+        <v>1.6099999999999996E-2</v>
+      </c>
+      <c r="F71" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C72">
-        <v>1.0101010101010104E-2</v>
+        <v>5.1652892561983479E-2</v>
       </c>
       <c r="D72" t="s">
         <v>76</v>
       </c>
       <c r="E72">
-        <v>0.65</v>
+        <v>4.0633333333333327E-2</v>
       </c>
       <c r="F72" t="s">
         <v>76</v>
@@ -9550,16 +9554,16 @@
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C73">
-        <v>1.2</v>
+        <v>1.0101010101010104E-2</v>
       </c>
       <c r="D73" t="s">
         <v>76</v>
       </c>
       <c r="E73">
-        <v>19.5</v>
+        <v>0.65</v>
       </c>
       <c r="F73" t="s">
         <v>76</v>
@@ -9567,16 +9571,16 @@
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>131</v>
-      </c>
-      <c r="C74" t="s">
-        <v>132</v>
+        <v>75</v>
+      </c>
+      <c r="C74">
+        <v>1.2</v>
       </c>
       <c r="D74" t="s">
-        <v>132</v>
+        <v>76</v>
       </c>
       <c r="E74">
-        <v>0.16866666666666666</v>
+        <v>19.5</v>
       </c>
       <c r="F74" t="s">
         <v>76</v>
@@ -9589,6 +9593,7 @@
     <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated total tRNA concentrations
</commit_message>
<xml_diff>
--- a/modeling/PURE Formulations.xlsx
+++ b/modeling/PURE Formulations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="560" windowWidth="21700" windowHeight="16120" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="3060" yWindow="460" windowWidth="21700" windowHeight="16120" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Literature PURE" sheetId="1" r:id="rId1"/>
@@ -233,6 +233,29 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
+    <comment ref="I2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+See next tab for predicted abundances
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E4" authorId="0">
       <text>
         <r>
@@ -255,7 +278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B26" authorId="0">
+    <comment ref="B41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -273,12 +296,33 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-See next tab for predicted abundances
-</t>
+Took Ile 1+2 calculation and divided by 2 since there is no way to distinguish between the 2 tRNAs' concentrations to my knowledge</t>
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0">
+    <comment ref="B43" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Took Leu1 calculation and divided by 2 since there is no way to distinguish between the 2 tRNAs' concentrations to my knowledge. (According to Conary's tRNA sheet, there is an extra leucine tRNA not included in this paper)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F78" authorId="0">
       <text>
         <r>
           <rPr>
@@ -300,7 +344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C73" authorId="0">
+    <comment ref="C118" authorId="0">
       <text>
         <r>
           <rPr>
@@ -381,7 +425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="139">
   <si>
     <t>PURE Component</t>
   </si>
@@ -789,6 +833,15 @@
   </si>
   <si>
     <t>2.16 µg/µL</t>
+  </si>
+  <si>
+    <t>Ile2</t>
+  </si>
+  <si>
+    <t>Ile1</t>
+  </si>
+  <si>
+    <t>LeuX</t>
   </si>
 </sst>
 </file>
@@ -912,6 +965,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -921,9 +977,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3983,11 +4036,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1185822176"/>
-        <c:axId val="1185824368"/>
+        <c:axId val="1191137872"/>
+        <c:axId val="1191140064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1185822176"/>
+        <c:axId val="1191137872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4110,7 +4163,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1185824368"/>
+        <c:crossAx val="1191140064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4118,7 +4171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1185824368"/>
+        <c:axId val="1191140064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4236,7 +4289,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1185822176"/>
+        <c:crossAx val="1191137872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5153,20 +5206,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -6427,22 +6480,22 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="3"/>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="K7" s="9"/>
+      <c r="K7" s="12"/>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
@@ -6919,7 +6972,7 @@
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="M26" s="10"/>
+      <c r="M26" s="7"/>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
@@ -6945,7 +6998,7 @@
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="M27" s="10"/>
+      <c r="M27" s="7"/>
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
@@ -6971,7 +7024,7 @@
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="M28" s="10"/>
+      <c r="M28" s="7"/>
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
@@ -7043,7 +7096,7 @@
         <v>25</v>
       </c>
       <c r="H31">
-        <f t="shared" ref="H31:H36" si="2">D31*1000</f>
+        <f t="shared" ref="H31:H34" si="2">D31*1000</f>
         <v>2000</v>
       </c>
       <c r="J31">
@@ -7293,7 +7346,7 @@
       <c r="E41" t="s">
         <v>34</v>
       </c>
-      <c r="F41" s="10">
+      <c r="F41" s="7">
         <v>96.36</v>
       </c>
       <c r="G41">
@@ -7322,11 +7375,11 @@
       <c r="E42" t="s">
         <v>34</v>
       </c>
-      <c r="F42" s="10">
+      <c r="F42" s="7">
         <v>63.47</v>
       </c>
       <c r="G42">
-        <f t="shared" ref="G42:G77" si="6">D42*6.0221366516752*10^20/(F42*1000)</f>
+        <f t="shared" ref="G42:G75" si="6">D42*6.0221366516752*10^20/(F42*1000)</f>
         <v>1.8976324725619032E+16</v>
       </c>
       <c r="H42">
@@ -7351,7 +7404,7 @@
       <c r="E43" t="s">
         <v>34</v>
       </c>
-      <c r="F43" s="10">
+      <c r="F43" s="7">
         <v>51.26</v>
       </c>
       <c r="G43">
@@ -7380,7 +7433,7 @@
       <c r="E44" t="s">
         <v>34</v>
       </c>
-      <c r="F44" s="10">
+      <c r="F44" s="7">
         <v>64.900000000000006</v>
       </c>
       <c r="G44">
@@ -7409,7 +7462,7 @@
       <c r="E45" t="s">
         <v>34</v>
       </c>
-      <c r="F45" s="10">
+      <c r="F45" s="7">
         <v>50.71</v>
       </c>
       <c r="G45">
@@ -7438,7 +7491,7 @@
       <c r="E46" t="s">
         <v>34</v>
       </c>
-      <c r="F46" s="10">
+      <c r="F46" s="7">
         <v>60.94</v>
       </c>
       <c r="G46">
@@ -7467,7 +7520,7 @@
       <c r="E47" t="s">
         <v>34</v>
       </c>
-      <c r="F47" s="10">
+      <c r="F47" s="7">
         <v>51.81</v>
       </c>
       <c r="G47">
@@ -7526,7 +7579,7 @@
       <c r="E49" t="s">
         <v>34</v>
       </c>
-      <c r="F49" s="10">
+      <c r="F49" s="7">
         <v>46.64</v>
       </c>
       <c r="G49">
@@ -7555,7 +7608,7 @@
       <c r="E50" t="s">
         <v>34</v>
       </c>
-      <c r="F50" s="10">
+      <c r="F50" s="7">
         <v>103.18</v>
       </c>
       <c r="G50">
@@ -7584,7 +7637,7 @@
       <c r="E51" t="s">
         <v>34</v>
       </c>
-      <c r="F51" s="10">
+      <c r="F51" s="7">
         <v>94.6</v>
       </c>
       <c r="G51">
@@ -7613,7 +7666,7 @@
       <c r="E52" t="s">
         <v>34</v>
       </c>
-      <c r="F52" s="10">
+      <c r="F52" s="7">
         <v>55.55</v>
       </c>
       <c r="G52">
@@ -7642,7 +7695,7 @@
       <c r="E53" t="s">
         <v>34</v>
       </c>
-      <c r="F53" s="10">
+      <c r="F53" s="7">
         <v>74.47</v>
       </c>
       <c r="G53">
@@ -7701,7 +7754,7 @@
       <c r="E55" t="s">
         <v>34</v>
       </c>
-      <c r="F55" s="10">
+      <c r="F55" s="7">
         <v>62.92</v>
       </c>
       <c r="G55">
@@ -7730,7 +7783,7 @@
       <c r="E56" t="s">
         <v>34</v>
       </c>
-      <c r="F56" s="10">
+      <c r="F56" s="7">
         <v>47.3</v>
       </c>
       <c r="G56">
@@ -7759,7 +7812,7 @@
       <c r="E57" t="s">
         <v>34</v>
       </c>
-      <c r="F57" s="10">
+      <c r="F57" s="7">
         <v>70.62</v>
       </c>
       <c r="G57">
@@ -7788,7 +7841,7 @@
       <c r="E58" t="s">
         <v>34</v>
       </c>
-      <c r="F58" s="10">
+      <c r="F58" s="7">
         <v>36.74</v>
       </c>
       <c r="G58">
@@ -7817,7 +7870,7 @@
       <c r="E59" t="s">
         <v>34</v>
       </c>
-      <c r="F59" s="10">
+      <c r="F59" s="7">
         <v>46.64</v>
       </c>
       <c r="G59">
@@ -7846,7 +7899,7 @@
       <c r="E60" t="s">
         <v>34</v>
       </c>
-      <c r="F60" s="10">
+      <c r="F60" s="7">
         <v>104.61</v>
       </c>
       <c r="G60">
@@ -7875,7 +7928,7 @@
       <c r="E61" t="s">
         <v>34</v>
       </c>
-      <c r="F61" s="10">
+      <c r="F61" s="7">
         <v>34.65</v>
       </c>
       <c r="G61">
@@ -7904,7 +7957,7 @@
       <c r="E62" t="s">
         <v>34</v>
       </c>
-      <c r="F62" s="10">
+      <c r="F62" s="7">
         <v>7.92</v>
       </c>
       <c r="G62">
@@ -7933,7 +7986,7 @@
       <c r="E63" t="s">
         <v>34</v>
       </c>
-      <c r="F63" s="10">
+      <c r="F63" s="7">
         <v>97.9</v>
       </c>
       <c r="G63">
@@ -7962,7 +8015,7 @@
       <c r="E64" t="s">
         <v>34</v>
       </c>
-      <c r="F64" s="10">
+      <c r="F64" s="7">
         <v>19.8</v>
       </c>
       <c r="G64">
@@ -7991,7 +8044,7 @@
       <c r="E65" t="s">
         <v>34</v>
       </c>
-      <c r="F65" s="10">
+      <c r="F65" s="7">
         <v>77.44</v>
       </c>
       <c r="G65">
@@ -8020,7 +8073,7 @@
       <c r="E66" t="s">
         <v>34</v>
       </c>
-      <c r="F66" s="10">
+      <c r="F66" s="7">
         <v>43.34</v>
       </c>
       <c r="G66">
@@ -8049,7 +8102,7 @@
       <c r="E67" t="s">
         <v>34</v>
       </c>
-      <c r="F67" s="10">
+      <c r="F67" s="7">
         <v>31.13</v>
       </c>
       <c r="G67">
@@ -8078,7 +8131,7 @@
       <c r="E68" t="s">
         <v>34</v>
       </c>
-      <c r="F68" s="11">
+      <c r="F68" s="8">
         <v>39.6</v>
       </c>
       <c r="G68">
@@ -8107,7 +8160,7 @@
       <c r="E69" t="s">
         <v>34</v>
       </c>
-      <c r="F69" s="11">
+      <c r="F69" s="8">
         <v>58.19</v>
       </c>
       <c r="G69">
@@ -8136,7 +8189,7 @@
       <c r="E70" t="s">
         <v>34</v>
       </c>
-      <c r="F70" s="10">
+      <c r="F70" s="7">
         <v>20.350000000000001</v>
       </c>
       <c r="G70">
@@ -8165,7 +8218,7 @@
       <c r="E71" t="s">
         <v>34</v>
       </c>
-      <c r="F71" s="10">
+      <c r="F71" s="7">
         <v>43.112000000000002</v>
       </c>
       <c r="G71">
@@ -8194,7 +8247,7 @@
       <c r="E72" t="s">
         <v>34</v>
       </c>
-      <c r="F72" s="10">
+      <c r="F72" s="7">
         <v>23.54</v>
       </c>
       <c r="G72">
@@ -8223,7 +8276,7 @@
       <c r="E73" t="s">
         <v>34</v>
       </c>
-      <c r="F73" s="10">
+      <c r="F73" s="7">
         <v>15.73</v>
       </c>
       <c r="G73">
@@ -8252,7 +8305,7 @@
       <c r="E74" t="s">
         <v>34</v>
       </c>
-      <c r="F74" s="10">
+      <c r="F74" s="7">
         <v>19.36</v>
       </c>
       <c r="G74">
@@ -8281,7 +8334,7 @@
       <c r="E75" t="s">
         <v>34</v>
       </c>
-      <c r="F75" s="10">
+      <c r="F75" s="7">
         <v>99</v>
       </c>
       <c r="G75">
@@ -8328,7 +8381,7 @@
       <c r="E77" t="s">
         <v>132</v>
       </c>
-      <c r="F77" s="10">
+      <c r="F77" s="7">
         <v>44</v>
       </c>
       <c r="G77">
@@ -8350,7 +8403,7 @@
       <c r="C82">
         <v>1</v>
       </c>
-      <c r="D82" s="12" t="s">
+      <c r="D82" s="9" t="s">
         <v>76</v>
       </c>
     </row>
@@ -8367,10 +8420,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F74"/>
+  <dimension ref="B2:M119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8380,23 +8433,40 @@
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C3" s="7" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2">
+        <v>84.58</v>
+      </c>
+      <c r="K2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2">
+        <v>939.79</v>
+      </c>
+      <c r="M2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C4" s="8" t="s">
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -8413,7 +8483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -8430,7 +8500,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -8447,7 +8517,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -8464,7 +8534,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -8481,7 +8551,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -8498,7 +8568,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -8515,7 +8585,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -8532,7 +8602,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -8549,7 +8619,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -8566,7 +8636,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -8583,7 +8653,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -8755,16 +8825,18 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="C26">
-        <v>84.58</v>
+        <f>'tRNA Abundances E. coli'!F56/100*$J$2</f>
+        <v>4.734620742539458</v>
       </c>
       <c r="D26" t="s">
         <v>76</v>
       </c>
       <c r="E26">
-        <v>939.79</v>
+        <f>'tRNA Abundances E. coli'!F56/100*$L$2</f>
+        <v>52.607581315099985</v>
       </c>
       <c r="F26" t="s">
         <v>76</v>
@@ -8772,16 +8844,18 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="C27">
-        <v>2000</v>
+        <f>'tRNA Abundances E. coli'!F57/100*$J$2</f>
+        <v>0.86206850277973024</v>
       </c>
       <c r="D27" t="s">
         <v>76</v>
       </c>
       <c r="E27">
-        <v>3750</v>
+        <f>'tRNA Abundances E. coli'!F57/100*$L$2</f>
+        <v>9.5786634928749432</v>
       </c>
       <c r="F27" t="s">
         <v>76</v>
@@ -8789,16 +8863,18 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="C28">
-        <v>2000</v>
+        <f>'tRNA Abundances E. coli'!F58/100*$J$2</f>
+        <v>6.4236264298038197</v>
       </c>
       <c r="D28" t="s">
         <v>76</v>
       </c>
       <c r="E28">
-        <v>2500</v>
+        <f>'tRNA Abundances E. coli'!F58/100*$L$2</f>
+        <v>71.374555243146503</v>
       </c>
       <c r="F28" t="s">
         <v>76</v>
@@ -8806,16 +8882,18 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="C29">
-        <v>1000</v>
+        <f>'tRNA Abundances E. coli'!F59/100*$J$2</f>
+        <v>0.61074445651479303</v>
       </c>
       <c r="D29" t="s">
         <v>76</v>
       </c>
       <c r="E29">
-        <v>1250</v>
+        <f>'tRNA Abundances E. coli'!F59/100*$L$2</f>
+        <v>6.7861377723816192</v>
       </c>
       <c r="F29" t="s">
         <v>76</v>
@@ -8823,16 +8901,18 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="C30">
-        <v>1000</v>
+        <f>'tRNA Abundances E. coli'!F60/100*$J$2</f>
+        <v>0.88098536647709091</v>
       </c>
       <c r="D30" t="s">
         <v>76</v>
       </c>
       <c r="E30">
-        <v>1250</v>
+        <f>'tRNA Abundances E. coli'!F60/100*$L$2</f>
+        <v>9.7888536008690625</v>
       </c>
       <c r="F30" t="s">
         <v>76</v>
@@ -8840,16 +8920,18 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="C31">
-        <v>20000</v>
+        <f>'tRNA Abundances E. coli'!F61/100*$J$2</f>
+        <v>0.66479263850725256</v>
       </c>
       <c r="D31" t="s">
         <v>76</v>
       </c>
       <c r="E31">
-        <v>25000</v>
+        <f>'tRNA Abundances E. coli'!F61/100*$L$2</f>
+        <v>7.3866809380791079</v>
       </c>
       <c r="F31" t="s">
         <v>76</v>
@@ -8857,16 +8939,18 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="C32">
-        <v>2.1121732995948852E-2</v>
+        <f>'tRNA Abundances E. coli'!F62/100*$J$2</f>
+        <v>1.6484695507700169</v>
       </c>
       <c r="D32" t="s">
         <v>76</v>
       </c>
       <c r="E32">
-        <v>2.1121732995948852E-2</v>
+        <f>'tRNA Abundances E. coli'!F62/100*$L$2</f>
+        <v>18.316566553773399</v>
       </c>
       <c r="F32" t="s">
         <v>76</v>
@@ -8874,16 +8958,18 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="C33">
-        <v>50000</v>
+        <f>'tRNA Abundances E. coli'!F63/100*$J$2</f>
+        <v>3.2537005559460659</v>
       </c>
       <c r="D33" t="s">
         <v>76</v>
       </c>
-      <c r="E33" t="s">
-        <v>132</v>
+      <c r="E33">
+        <f>'tRNA Abundances E. coli'!F63/100*$L$2</f>
+        <v>36.152698574988804</v>
       </c>
       <c r="F33" t="s">
         <v>76</v>
@@ -8891,16 +8977,18 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="C34">
-        <v>100000</v>
+        <f>'tRNA Abundances E. coli'!F64/100*$J$2</f>
+        <v>1.9024960061345768</v>
       </c>
       <c r="D34" t="s">
         <v>76</v>
       </c>
       <c r="E34">
-        <v>280000</v>
+        <f>'tRNA Abundances E. coli'!F64/100*$L$2</f>
+        <v>21.139119432551595</v>
       </c>
       <c r="F34" t="s">
         <v>76</v>
@@ -8908,16 +8996,18 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="C35">
-        <v>13000</v>
+        <f>'tRNA Abundances E. coli'!F65/100*$J$2</f>
+        <v>0.85666368458048414</v>
       </c>
       <c r="D35" t="s">
         <v>76</v>
       </c>
       <c r="E35">
-        <v>24500</v>
+        <f>'tRNA Abundances E. coli'!F65/100*$L$2</f>
+        <v>9.5186091763051923</v>
       </c>
       <c r="F35" t="s">
         <v>76</v>
@@ -8925,16 +9015,18 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="C36">
-        <v>2000</v>
+        <f>'tRNA Abundances E. coli'!F66/100*$J$2</f>
+        <v>1.3701214135088502</v>
       </c>
       <c r="D36" t="s">
         <v>76</v>
       </c>
       <c r="E36">
-        <v>1500</v>
+        <f>'tRNA Abundances E. coli'!F66/100*$L$2</f>
+        <v>15.223769250431335</v>
       </c>
       <c r="F36" t="s">
         <v>76</v>
@@ -8942,16 +9034,18 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="C37">
-        <v>1000</v>
+        <f>'tRNA Abundances E. coli'!F67/100*$J$2</f>
+        <v>6.518210748290624</v>
       </c>
       <c r="D37" t="s">
         <v>76</v>
       </c>
       <c r="E37">
-        <v>1500</v>
+        <f>'tRNA Abundances E. coli'!F67/100*$L$2</f>
+        <v>72.425505783117117</v>
       </c>
       <c r="F37" t="s">
         <v>76</v>
@@ -8959,16 +9053,18 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="C38">
-        <v>0.71606475716064766</v>
+        <f>'tRNA Abundances E. coli'!F68/100*$J$2</f>
+        <v>2.9591379640871613</v>
       </c>
       <c r="D38" t="s">
         <v>76</v>
       </c>
       <c r="E38">
-        <v>0.72833333333333328</v>
+        <f>'tRNA Abundances E. coli'!F68/100*$L$2</f>
+        <v>32.879738321937495</v>
       </c>
       <c r="F38" t="s">
         <v>76</v>
@@ -8976,16 +9072,18 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="C39">
-        <v>3.1510950055144163E-2</v>
+        <f>'tRNA Abundances E. coli'!F69/100*$J$2</f>
+        <v>5.3615796536519893</v>
       </c>
       <c r="D39" t="s">
         <v>76</v>
       </c>
       <c r="E39">
-        <v>3.0666666666666665E-2</v>
+        <f>'tRNA Abundances E. coli'!F69/100*$L$2</f>
+        <v>59.573882037190863</v>
       </c>
       <c r="F39" t="s">
         <v>76</v>
@@ -8993,16 +9091,18 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="C40">
-        <v>0.42918454935622319</v>
+        <f>'tRNA Abundances E. coli'!F70/100*$J$2</f>
+        <v>0.9053070483736978</v>
       </c>
       <c r="D40" t="s">
         <v>76</v>
       </c>
       <c r="E40">
-        <v>0.42166666666666663</v>
+        <f>'tRNA Abundances E. coli'!F70/100*$L$2</f>
+        <v>10.059098025432933</v>
       </c>
       <c r="F40" t="s">
         <v>76</v>
@@ -9010,16 +9110,18 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="C41">
-        <v>0.12326656394453005</v>
+        <f>5.11295801648668/2</f>
+        <v>2.5564790082433402</v>
       </c>
       <c r="D41" t="s">
         <v>76</v>
       </c>
       <c r="E41">
-        <v>0.12266666666666666</v>
+        <f>56.8113834749824/2</f>
+        <v>28.4056917374912</v>
       </c>
       <c r="F41" t="s">
         <v>76</v>
@@ -9027,16 +9129,18 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="C42">
-        <v>2.3663971603234076E-2</v>
+        <f>5.11295801648668/2</f>
+        <v>2.5564790082433402</v>
       </c>
       <c r="D42" t="s">
         <v>76</v>
       </c>
       <c r="E42">
-        <v>2.3766666666666665E-2</v>
+        <f>56.8113834749824/2</f>
+        <v>28.4056917374912</v>
       </c>
       <c r="F42" t="s">
         <v>76</v>
@@ -9044,16 +9148,18 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>45</v>
+        <v>138</v>
       </c>
       <c r="C43">
-        <v>6.2356416147029865E-2</v>
+        <f>5.76153620039619/2</f>
+        <v>2.8807681001980949</v>
       </c>
       <c r="D43" t="s">
         <v>76</v>
       </c>
       <c r="E43">
-        <v>5.9799999999999992E-2</v>
+        <f>64.0179014633523/2</f>
+        <v>32.008950731676151</v>
       </c>
       <c r="F43" t="s">
         <v>76</v>
@@ -9061,16 +9167,18 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="C44">
-        <v>0.24319629415170818</v>
+        <f>5.76153620039619/2</f>
+        <v>2.8807681001980949</v>
       </c>
       <c r="D44" t="s">
         <v>76</v>
       </c>
       <c r="E44">
-        <v>0.22999999999999998</v>
+        <f>64.0179014633523/2</f>
+        <v>32.008950731676151</v>
       </c>
       <c r="F44" t="s">
         <v>76</v>
@@ -9078,16 +9186,18 @@
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="C45">
-        <v>8.797653958944282E-2</v>
+        <f>'tRNA Abundances E. coli'!F73/100*$J$2</f>
+        <v>1.2755370950220457</v>
       </c>
       <c r="D45" t="s">
         <v>76</v>
       </c>
       <c r="E45">
-        <v>8.433333333333333E-2</v>
+        <f>'tRNA Abundances E. coli'!F73/100*$L$2</f>
+        <v>14.172818710460728</v>
       </c>
       <c r="F45" t="s">
         <v>76</v>
@@ -9095,16 +9205,18 @@
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="C46">
-        <v>1.7152658662092625E-2</v>
+        <f>'tRNA Abundances E. coli'!F74/100*$J$2</f>
+        <v>0.86206850277973024</v>
       </c>
       <c r="D46" t="s">
         <v>76</v>
       </c>
       <c r="E46">
-        <v>8.433333333333333E-2</v>
+        <f>'tRNA Abundances E. coli'!F74/100*$L$2</f>
+        <v>9.5786634928749432</v>
       </c>
       <c r="F46" t="s">
         <v>76</v>
@@ -9112,16 +9224,18 @@
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="C47">
-        <v>0.38767202946307433</v>
+        <f>'tRNA Abundances E. coli'!F75/100*$J$2</f>
+        <v>2.6105271902357972</v>
       </c>
       <c r="D47" t="s">
         <v>76</v>
       </c>
       <c r="E47">
-        <v>0.36799999999999999</v>
+        <f>'tRNA Abundances E. coli'!F75/100*$L$2</f>
+        <v>29.006234903188691</v>
       </c>
       <c r="F47" t="s">
         <v>76</v>
@@ -9129,16 +9243,18 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="C48">
-        <v>4.22832980972516E-2</v>
+        <f>'tRNA Abundances E. coli'!F76/100*$J$2</f>
+        <v>0.98637932136238726</v>
       </c>
       <c r="D48" t="s">
         <v>76</v>
       </c>
       <c r="E48">
-        <v>4.0633333333333327E-2</v>
+        <f>'tRNA Abundances E. coli'!F76/100*$L$2</f>
+        <v>10.959912773979166</v>
       </c>
       <c r="F48" t="s">
         <v>76</v>
@@ -9146,16 +9262,18 @@
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>51</v>
+        <v>105</v>
       </c>
       <c r="C49">
-        <v>0.11521152115211523</v>
+        <f>'tRNA Abundances E. coli'!F77/100*$J$2</f>
+        <v>2.3592031439708605</v>
       </c>
       <c r="D49" t="s">
         <v>76</v>
       </c>
       <c r="E49">
-        <v>0.11499999999999999</v>
+        <f>'tRNA Abundances E. coli'!F77/100*$L$2</f>
+        <v>26.213709182695375</v>
       </c>
       <c r="F49" t="s">
         <v>76</v>
@@ -9163,16 +9281,18 @@
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="C50">
-        <v>2.819927487578891E-2</v>
+        <f>'tRNA Abundances E. coli'!F78/100*$J$2</f>
+        <v>1.7106249600613452</v>
       </c>
       <c r="D50" t="s">
         <v>76</v>
       </c>
       <c r="E50">
-        <v>0.10733333333333332</v>
+        <f>'tRNA Abundances E. coli'!F78/100*$L$2</f>
+        <v>19.007191194325511</v>
       </c>
       <c r="F50" t="s">
         <v>76</v>
@@ -9180,16 +9300,18 @@
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="C51">
-        <v>0.13774104683195595</v>
+        <f>'tRNA Abundances E. coli'!F79/100*$J$2</f>
+        <v>0.91341427567256661</v>
       </c>
       <c r="D51" t="s">
         <v>76</v>
       </c>
       <c r="E51">
-        <v>0.13033333333333333</v>
+        <f>'tRNA Abundances E. coli'!F79/100*$L$2</f>
+        <v>10.149179500287556</v>
       </c>
       <c r="F51" t="s">
         <v>76</v>
@@ -9197,16 +9319,18 @@
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C52">
-        <v>0.15893197711379531</v>
+        <f>'tRNA Abundances E. coli'!F80/100*$J$2</f>
+        <v>1.1079877308454209</v>
       </c>
       <c r="D52" t="s">
         <v>76</v>
       </c>
       <c r="E52">
-        <v>0.16866666666666666</v>
+        <f>'tRNA Abundances E. coli'!F80/100*$L$2</f>
+        <v>12.311134896798512</v>
       </c>
       <c r="F52" t="s">
         <v>76</v>
@@ -9214,16 +9338,18 @@
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="C53">
-        <v>4.0169133192389003E-2</v>
+        <f>'tRNA Abundances E. coli'!F81/100*$J$2</f>
+        <v>1.2674298677231772</v>
       </c>
       <c r="D53" t="s">
         <v>76</v>
       </c>
       <c r="E53">
-        <v>7.6666666666666661E-2</v>
+        <f>'tRNA Abundances E. coli'!F81/100*$L$2</f>
+        <v>14.082737235606109</v>
       </c>
       <c r="F53" t="s">
         <v>76</v>
@@ -9231,16 +9357,18 @@
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="C54">
-        <v>8.9209855564995763E-2</v>
+        <f>'tRNA Abundances E. coli'!F82/100*$J$2</f>
+        <v>0.74316250239631909</v>
       </c>
       <c r="D54" t="s">
         <v>76</v>
       </c>
       <c r="E54">
-        <v>8.433333333333333E-2</v>
+        <f>'tRNA Abundances E. coli'!F82/100*$L$2</f>
+        <v>8.2574685283404676</v>
       </c>
       <c r="F54" t="s">
         <v>76</v>
@@ -9248,16 +9376,18 @@
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="C55">
-        <v>2.9940119760479045E-2</v>
+        <f>'tRNA Abundances E. coli'!F83/100*$J$2</f>
+        <v>1.0836660489488144</v>
       </c>
       <c r="D55" t="s">
         <v>76</v>
       </c>
       <c r="E55">
-        <v>2.8366666666666665E-2</v>
+        <f>'tRNA Abundances E. coli'!F83/100*$L$2</f>
+        <v>12.040890472234645</v>
       </c>
       <c r="F55" t="s">
         <v>76</v>
@@ -9265,16 +9395,18 @@
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="C56">
-        <v>1.2864493996569469E-2</v>
+        <f>'tRNA Abundances E. coli'!F84/100*$J$2</f>
+        <v>0.68911432040385934</v>
       </c>
       <c r="D56" t="s">
         <v>76</v>
       </c>
       <c r="E56">
-        <v>0.15333333333333332</v>
+        <f>'tRNA Abundances E. coli'!F84/100*$L$2</f>
+        <v>7.6569253626429772</v>
       </c>
       <c r="F56" t="s">
         <v>76</v>
@@ -9282,16 +9414,18 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="C57">
-        <v>1.7206767995411532E-2</v>
+        <f>'tRNA Abundances E. coli'!F85/100*$J$2</f>
+        <v>0.28375295546041274</v>
       </c>
       <c r="D57" t="s">
         <v>76</v>
       </c>
       <c r="E57">
-        <v>1.6866666666666665E-2</v>
+        <f>'tRNA Abundances E. coli'!F85/100*$L$2</f>
+        <v>3.1528516199118144</v>
       </c>
       <c r="F57" t="s">
         <v>76</v>
@@ -9299,16 +9433,18 @@
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="C58">
-        <v>0.57720057720057727</v>
+        <f>'tRNA Abundances E. coli'!F86/100*$J$2</f>
+        <v>1.886281551536839</v>
       </c>
       <c r="D58" t="s">
         <v>76</v>
       </c>
       <c r="E58">
-        <v>0.59033333333333327</v>
+        <f>'tRNA Abundances E. coli'!F86/100*$L$2</f>
+        <v>20.95895648284235</v>
       </c>
       <c r="F58" t="s">
         <v>76</v>
@@ -9316,16 +9452,18 @@
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="C59">
-        <v>1.2626262626262628</v>
+        <f>'tRNA Abundances E. coli'!F87/100*$J$2</f>
+        <v>0.37023004664834802</v>
       </c>
       <c r="D59" t="s">
         <v>76</v>
       </c>
       <c r="E59">
-        <v>24.533333333333335</v>
+        <f>'tRNA Abundances E. coli'!F87/100*$L$2</f>
+        <v>4.1137206850277961</v>
       </c>
       <c r="F59" t="s">
         <v>76</v>
@@ -9333,16 +9471,18 @@
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="C60">
-        <v>0.4085801838610828</v>
+        <f>'tRNA Abundances E. coli'!F88/100*$J$2</f>
+        <v>1.4593009137964084</v>
       </c>
       <c r="D60" t="s">
         <v>76</v>
       </c>
       <c r="E60">
-        <v>0.99666666666666659</v>
+        <f>'tRNA Abundances E. coli'!F88/100*$L$2</f>
+        <v>16.214665473832191</v>
       </c>
       <c r="F60" t="s">
         <v>76</v>
@@ -9350,16 +9490,18 @@
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="C61">
-        <v>0.50505050505050508</v>
+        <f>'tRNA Abundances E. coli'!F89/100*$J$2</f>
+        <v>0.99448654866125619</v>
       </c>
       <c r="D61" t="s">
         <v>76</v>
       </c>
       <c r="E61">
-        <v>1.2266666666666666</v>
+        <f>'tRNA Abundances E. coli'!F89/100*$L$2</f>
+        <v>11.049994248833789</v>
       </c>
       <c r="F61" t="s">
         <v>76</v>
@@ -9367,16 +9509,18 @@
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="C62">
-        <v>0.64566115702479332</v>
+        <f>'tRNA Abundances E. coli'!F90/100*$J$2</f>
+        <v>0.15133490957888682</v>
       </c>
       <c r="D62" t="s">
         <v>76</v>
       </c>
       <c r="E62">
-        <v>1.0733333333333333</v>
+        <f>'tRNA Abundances E. coli'!F90/100*$L$2</f>
+        <v>1.681520863952968</v>
       </c>
       <c r="F62" t="s">
         <v>76</v>
@@ -9384,16 +9528,18 @@
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C63">
-        <v>2.3073373327180429</v>
+        <f>'tRNA Abundances E. coli'!F91/100*$J$2</f>
+        <v>0.72154322959933526</v>
       </c>
       <c r="D63" t="s">
         <v>76</v>
       </c>
       <c r="E63">
-        <v>7.6666666666666661</v>
+        <f>'tRNA Abundances E. coli'!F91/100*$L$2</f>
+        <v>8.0172512620614711</v>
       </c>
       <c r="F63" t="s">
         <v>76</v>
@@ -9401,16 +9547,18 @@
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="C64">
-        <v>1.6061676839061996</v>
+        <f>'tRNA Abundances E. coli'!F92/100*$J$2</f>
+        <v>1.3133708224167675</v>
       </c>
       <c r="D64" t="s">
         <v>76</v>
       </c>
       <c r="E64">
-        <v>3.2966666666666664</v>
+        <f>'tRNA Abundances E. coli'!F92/100*$L$2</f>
+        <v>14.593198926448972</v>
       </c>
       <c r="F64" t="s">
         <v>76</v>
@@ -9418,16 +9566,18 @@
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="C65">
-        <v>0.25252525252525254</v>
+        <f>'tRNA Abundances E. coli'!F93/100*$J$2</f>
+        <v>1.3485021407118662</v>
       </c>
       <c r="D65" t="s">
         <v>76</v>
       </c>
       <c r="E65">
-        <v>4.9066666666666668E-2</v>
+        <f>'tRNA Abundances E. coli'!F93/100*$L$2</f>
+        <v>14.983551984152337</v>
       </c>
       <c r="F65" t="s">
         <v>76</v>
@@ -9435,16 +9585,18 @@
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>131</v>
-      </c>
-      <c r="C66" t="s">
-        <v>132</v>
+        <v>122</v>
+      </c>
+      <c r="C66">
+        <f>'tRNA Abundances E. coli'!F94/100*$J$2</f>
+        <v>1.1214997763435361</v>
       </c>
       <c r="D66" t="s">
-        <v>132</v>
+        <v>76</v>
       </c>
       <c r="E66">
-        <v>0.16866666666666666</v>
+        <f>'tRNA Abundances E. coli'!F94/100*$L$2</f>
+        <v>12.461270688222887</v>
       </c>
       <c r="F66" t="s">
         <v>76</v>
@@ -9452,16 +9604,18 @@
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="C67">
-        <v>0.1718508334765424</v>
+        <f>'tRNA Abundances E. coli'!F95/100*$J$2</f>
+        <v>1.2458105949261931</v>
       </c>
       <c r="D67" t="s">
         <v>76</v>
       </c>
       <c r="E67">
-        <v>0.16866666666666666</v>
+        <f>'tRNA Abundances E. coli'!F95/100*$L$2</f>
+        <v>13.84251996932711</v>
       </c>
       <c r="F67" t="s">
         <v>76</v>
@@ -9469,16 +9623,18 @@
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="C68">
-        <v>0.49140049140049158</v>
+        <f>'tRNA Abundances E. coli'!F96/100*$J$2</f>
+        <v>1.4106575500031946</v>
       </c>
       <c r="D68" t="s">
         <v>76</v>
       </c>
       <c r="E68">
-        <v>3.9099999999999997</v>
+        <f>'tRNA Abundances E. coli'!F96/100*$L$2</f>
+        <v>15.674176624704447</v>
       </c>
       <c r="F68" t="s">
         <v>76</v>
@@ -9486,16 +9642,18 @@
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="C69">
-        <v>9.2781592132120991E-2</v>
+        <f>'tRNA Abundances E. coli'!F97/100*$J$2</f>
+        <v>5.1318748801840348</v>
       </c>
       <c r="D69" t="s">
         <v>76</v>
       </c>
       <c r="E69">
-        <v>0.24533333333333332</v>
+        <f>'tRNA Abundances E. coli'!F97/100*$L$2</f>
+        <v>57.021573582976522</v>
       </c>
       <c r="F69" t="s">
         <v>76</v>
@@ -9503,16 +9661,18 @@
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="C70">
-        <v>0.12744265080713679</v>
+        <f>'tRNA Abundances E. coli'!F98/100*$J$2</f>
+        <v>0.72965045689820418</v>
       </c>
       <c r="D70" t="s">
         <v>76</v>
       </c>
       <c r="E70">
-        <v>1.38</v>
+        <f>'tRNA Abundances E. coli'!F98/100*$L$2</f>
+        <v>8.1073327369160957</v>
       </c>
       <c r="F70" t="s">
         <v>76</v>
@@ -9520,16 +9680,18 @@
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="C71">
-        <v>6.9930069930069963E-2</v>
+        <f>'tRNA Abundances E. coli'!F99/100*$J$2</f>
+        <v>0.9755696849638954</v>
       </c>
       <c r="D71" t="s">
         <v>76</v>
       </c>
       <c r="E71">
-        <v>1.6099999999999996E-2</v>
+        <f>'tRNA Abundances E. coli'!F99/100*$L$2</f>
+        <v>10.83980414083967</v>
       </c>
       <c r="F71" t="s">
         <v>76</v>
@@ -9537,16 +9699,16 @@
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="C72">
-        <v>5.1652892561983479E-2</v>
+        <v>2000</v>
       </c>
       <c r="D72" t="s">
         <v>76</v>
       </c>
       <c r="E72">
-        <v>4.0633333333333327E-2</v>
+        <v>3750</v>
       </c>
       <c r="F72" t="s">
         <v>76</v>
@@ -9554,16 +9716,16 @@
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="C73">
-        <v>1.0101010101010104E-2</v>
+        <v>2000</v>
       </c>
       <c r="D73" t="s">
         <v>76</v>
       </c>
       <c r="E73">
-        <v>0.65</v>
+        <v>2500</v>
       </c>
       <c r="F73" t="s">
         <v>76</v>
@@ -9571,18 +9733,783 @@
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
+        <v>30</v>
+      </c>
+      <c r="C74">
+        <v>1000</v>
+      </c>
+      <c r="D74" t="s">
+        <v>76</v>
+      </c>
+      <c r="E74">
+        <v>1250</v>
+      </c>
+      <c r="F74" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>31</v>
+      </c>
+      <c r="C75">
+        <v>1000</v>
+      </c>
+      <c r="D75" t="s">
+        <v>76</v>
+      </c>
+      <c r="E75">
+        <v>1250</v>
+      </c>
+      <c r="F75" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>32</v>
+      </c>
+      <c r="C76">
+        <v>20000</v>
+      </c>
+      <c r="D76" t="s">
+        <v>76</v>
+      </c>
+      <c r="E76">
+        <v>25000</v>
+      </c>
+      <c r="F76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>33</v>
+      </c>
+      <c r="C77">
+        <v>2.1121732995948852E-2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>76</v>
+      </c>
+      <c r="E77">
+        <v>2.1121732995948852E-2</v>
+      </c>
+      <c r="F77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>35</v>
+      </c>
+      <c r="C78">
+        <v>50000</v>
+      </c>
+      <c r="D78" t="s">
+        <v>76</v>
+      </c>
+      <c r="E78" t="s">
+        <v>132</v>
+      </c>
+      <c r="F78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C79">
+        <v>100000</v>
+      </c>
+      <c r="D79" t="s">
+        <v>76</v>
+      </c>
+      <c r="E79">
+        <v>280000</v>
+      </c>
+      <c r="F79" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>37</v>
+      </c>
+      <c r="C80">
+        <v>13000</v>
+      </c>
+      <c r="D80" t="s">
+        <v>76</v>
+      </c>
+      <c r="E80">
+        <v>24500</v>
+      </c>
+      <c r="F80" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>38</v>
+      </c>
+      <c r="C81">
+        <v>2000</v>
+      </c>
+      <c r="D81" t="s">
+        <v>76</v>
+      </c>
+      <c r="E81">
+        <v>1500</v>
+      </c>
+      <c r="F81" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>39</v>
+      </c>
+      <c r="C82">
+        <v>1000</v>
+      </c>
+      <c r="D82" t="s">
+        <v>76</v>
+      </c>
+      <c r="E82">
+        <v>1500</v>
+      </c>
+      <c r="F82" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83">
+        <v>0.71606475716064766</v>
+      </c>
+      <c r="D83" t="s">
+        <v>76</v>
+      </c>
+      <c r="E83">
+        <v>0.72833333333333328</v>
+      </c>
+      <c r="F83" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>41</v>
+      </c>
+      <c r="C84">
+        <v>3.1510950055144163E-2</v>
+      </c>
+      <c r="D84" t="s">
+        <v>76</v>
+      </c>
+      <c r="E84">
+        <v>3.0666666666666665E-2</v>
+      </c>
+      <c r="F84" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85">
+        <v>0.42918454935622319</v>
+      </c>
+      <c r="D85" t="s">
+        <v>76</v>
+      </c>
+      <c r="E85">
+        <v>0.42166666666666663</v>
+      </c>
+      <c r="F85" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
+        <v>43</v>
+      </c>
+      <c r="C86">
+        <v>0.12326656394453005</v>
+      </c>
+      <c r="D86" t="s">
+        <v>76</v>
+      </c>
+      <c r="E86">
+        <v>0.12266666666666666</v>
+      </c>
+      <c r="F86" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>44</v>
+      </c>
+      <c r="C87">
+        <v>2.3663971603234076E-2</v>
+      </c>
+      <c r="D87" t="s">
+        <v>76</v>
+      </c>
+      <c r="E87">
+        <v>2.3766666666666665E-2</v>
+      </c>
+      <c r="F87" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>45</v>
+      </c>
+      <c r="C88">
+        <v>6.2356416147029865E-2</v>
+      </c>
+      <c r="D88" t="s">
+        <v>76</v>
+      </c>
+      <c r="E88">
+        <v>5.9799999999999992E-2</v>
+      </c>
+      <c r="F88" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>46</v>
+      </c>
+      <c r="C89">
+        <v>0.24319629415170818</v>
+      </c>
+      <c r="D89" t="s">
+        <v>76</v>
+      </c>
+      <c r="E89">
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="F89" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
+        <v>47</v>
+      </c>
+      <c r="C90">
+        <v>8.797653958944282E-2</v>
+      </c>
+      <c r="D90" t="s">
+        <v>76</v>
+      </c>
+      <c r="E90">
+        <v>8.433333333333333E-2</v>
+      </c>
+      <c r="F90" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>48</v>
+      </c>
+      <c r="C91">
+        <v>1.7152658662092625E-2</v>
+      </c>
+      <c r="D91" t="s">
+        <v>76</v>
+      </c>
+      <c r="E91">
+        <v>8.433333333333333E-2</v>
+      </c>
+      <c r="F91" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>49</v>
+      </c>
+      <c r="C92">
+        <v>0.38767202946307433</v>
+      </c>
+      <c r="D92" t="s">
+        <v>76</v>
+      </c>
+      <c r="E92">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="F92" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>50</v>
+      </c>
+      <c r="C93">
+        <v>4.22832980972516E-2</v>
+      </c>
+      <c r="D93" t="s">
+        <v>76</v>
+      </c>
+      <c r="E93">
+        <v>4.0633333333333327E-2</v>
+      </c>
+      <c r="F93" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>51</v>
+      </c>
+      <c r="C94">
+        <v>0.11521152115211523</v>
+      </c>
+      <c r="D94" t="s">
+        <v>76</v>
+      </c>
+      <c r="E94">
+        <v>0.11499999999999999</v>
+      </c>
+      <c r="F94" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>52</v>
+      </c>
+      <c r="C95">
+        <v>2.819927487578891E-2</v>
+      </c>
+      <c r="D95" t="s">
+        <v>76</v>
+      </c>
+      <c r="E95">
+        <v>0.10733333333333332</v>
+      </c>
+      <c r="F95" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>53</v>
+      </c>
+      <c r="C96">
+        <v>0.13774104683195595</v>
+      </c>
+      <c r="D96" t="s">
+        <v>76</v>
+      </c>
+      <c r="E96">
+        <v>0.13033333333333333</v>
+      </c>
+      <c r="F96" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>54</v>
+      </c>
+      <c r="C97">
+        <v>0.15893197711379531</v>
+      </c>
+      <c r="D97" t="s">
+        <v>76</v>
+      </c>
+      <c r="E97">
+        <v>0.16866666666666666</v>
+      </c>
+      <c r="F97" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>55</v>
+      </c>
+      <c r="C98">
+        <v>4.0169133192389003E-2</v>
+      </c>
+      <c r="D98" t="s">
+        <v>76</v>
+      </c>
+      <c r="E98">
+        <v>7.6666666666666661E-2</v>
+      </c>
+      <c r="F98" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C99">
+        <v>8.9209855564995763E-2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>76</v>
+      </c>
+      <c r="E99">
+        <v>8.433333333333333E-2</v>
+      </c>
+      <c r="F99" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>57</v>
+      </c>
+      <c r="C100">
+        <v>2.9940119760479045E-2</v>
+      </c>
+      <c r="D100" t="s">
+        <v>76</v>
+      </c>
+      <c r="E100">
+        <v>2.8366666666666665E-2</v>
+      </c>
+      <c r="F100" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>58</v>
+      </c>
+      <c r="C101">
+        <v>1.2864493996569469E-2</v>
+      </c>
+      <c r="D101" t="s">
+        <v>76</v>
+      </c>
+      <c r="E101">
+        <v>0.15333333333333332</v>
+      </c>
+      <c r="F101" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>59</v>
+      </c>
+      <c r="C102">
+        <v>1.7206767995411532E-2</v>
+      </c>
+      <c r="D102" t="s">
+        <v>76</v>
+      </c>
+      <c r="E102">
+        <v>1.6866666666666665E-2</v>
+      </c>
+      <c r="F102" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>60</v>
+      </c>
+      <c r="C103">
+        <v>0.57720057720057727</v>
+      </c>
+      <c r="D103" t="s">
+        <v>76</v>
+      </c>
+      <c r="E103">
+        <v>0.59033333333333327</v>
+      </c>
+      <c r="F103" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
+        <v>61</v>
+      </c>
+      <c r="C104">
+        <v>1.2626262626262628</v>
+      </c>
+      <c r="D104" t="s">
+        <v>76</v>
+      </c>
+      <c r="E104">
+        <v>24.533333333333335</v>
+      </c>
+      <c r="F104" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>62</v>
+      </c>
+      <c r="C105">
+        <v>0.4085801838610828</v>
+      </c>
+      <c r="D105" t="s">
+        <v>76</v>
+      </c>
+      <c r="E105">
+        <v>0.99666666666666659</v>
+      </c>
+      <c r="F105" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>63</v>
+      </c>
+      <c r="C106">
+        <v>0.50505050505050508</v>
+      </c>
+      <c r="D106" t="s">
+        <v>76</v>
+      </c>
+      <c r="E106">
+        <v>1.2266666666666666</v>
+      </c>
+      <c r="F106" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>64</v>
+      </c>
+      <c r="C107">
+        <v>0.64566115702479332</v>
+      </c>
+      <c r="D107" t="s">
+        <v>76</v>
+      </c>
+      <c r="E107">
+        <v>1.0733333333333333</v>
+      </c>
+      <c r="F107" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>65</v>
+      </c>
+      <c r="C108">
+        <v>2.3073373327180429</v>
+      </c>
+      <c r="D108" t="s">
+        <v>76</v>
+      </c>
+      <c r="E108">
+        <v>7.6666666666666661</v>
+      </c>
+      <c r="F108" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>66</v>
+      </c>
+      <c r="C109">
+        <v>1.6061676839061996</v>
+      </c>
+      <c r="D109" t="s">
+        <v>76</v>
+      </c>
+      <c r="E109">
+        <v>3.2966666666666664</v>
+      </c>
+      <c r="F109" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>67</v>
+      </c>
+      <c r="C110">
+        <v>0.25252525252525254</v>
+      </c>
+      <c r="D110" t="s">
+        <v>76</v>
+      </c>
+      <c r="E110">
+        <v>4.9066666666666668E-2</v>
+      </c>
+      <c r="F110" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>131</v>
+      </c>
+      <c r="C111" t="s">
+        <v>132</v>
+      </c>
+      <c r="D111" t="s">
+        <v>132</v>
+      </c>
+      <c r="E111">
+        <v>0.16866666666666666</v>
+      </c>
+      <c r="F111" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B112" t="s">
+        <v>68</v>
+      </c>
+      <c r="C112">
+        <v>0.1718508334765424</v>
+      </c>
+      <c r="D112" t="s">
+        <v>76</v>
+      </c>
+      <c r="E112">
+        <v>0.16866666666666666</v>
+      </c>
+      <c r="F112" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
+        <v>69</v>
+      </c>
+      <c r="C113">
+        <v>0.49140049140049158</v>
+      </c>
+      <c r="D113" t="s">
+        <v>76</v>
+      </c>
+      <c r="E113">
+        <v>3.9099999999999997</v>
+      </c>
+      <c r="F113" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>70</v>
+      </c>
+      <c r="C114">
+        <v>9.2781592132120991E-2</v>
+      </c>
+      <c r="D114" t="s">
+        <v>76</v>
+      </c>
+      <c r="E114">
+        <v>0.24533333333333332</v>
+      </c>
+      <c r="F114" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B115" t="s">
+        <v>71</v>
+      </c>
+      <c r="C115">
+        <v>0.12744265080713679</v>
+      </c>
+      <c r="D115" t="s">
+        <v>76</v>
+      </c>
+      <c r="E115">
+        <v>1.38</v>
+      </c>
+      <c r="F115" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C116">
+        <v>6.9930069930069963E-2</v>
+      </c>
+      <c r="D116" t="s">
+        <v>76</v>
+      </c>
+      <c r="E116">
+        <v>1.6099999999999996E-2</v>
+      </c>
+      <c r="F116" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B117" t="s">
+        <v>73</v>
+      </c>
+      <c r="C117">
+        <v>5.1652892561983479E-2</v>
+      </c>
+      <c r="D117" t="s">
+        <v>76</v>
+      </c>
+      <c r="E117">
+        <v>4.0633333333333327E-2</v>
+      </c>
+      <c r="F117" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
+        <v>74</v>
+      </c>
+      <c r="C118">
+        <v>1.0101010101010104E-2</v>
+      </c>
+      <c r="D118" t="s">
+        <v>76</v>
+      </c>
+      <c r="E118">
+        <v>0.65</v>
+      </c>
+      <c r="F118" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B119" t="s">
         <v>75</v>
       </c>
-      <c r="C74">
+      <c r="C119">
         <v>1.2</v>
       </c>
-      <c r="D74" t="s">
-        <v>76</v>
-      </c>
-      <c r="E74">
+      <c r="D119" t="s">
+        <v>76</v>
+      </c>
+      <c r="E119">
         <v>19.5</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F119" t="s">
         <v>76</v>
       </c>
     </row>
@@ -9602,8 +10529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>